<commit_message>
update mergesort using ForkJoinPool
</commit_message>
<xml_diff>
--- a/Sort_Unit_Test.xlsx
+++ b/Sort_Unit_Test.xlsx
@@ -4,44 +4,51 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16935" windowHeight="8400"/>
+    <workbookView windowWidth="28800" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$6</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Avg</t>
+    <t>Avg (second)</t>
   </si>
   <si>
-    <t>Quick Sort</t>
+    <t>Array.parallelSort()</t>
   </si>
   <si>
     <t>ForkJoinPool and QuickSort</t>
   </si>
   <si>
+    <t>ForkJoinPool and MergeSort</t>
+  </si>
+  <si>
     <t>Array.sort()</t>
   </si>
   <si>
-    <t>Array.parallelSort()</t>
+    <t>Quick Sort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,8 +57,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -507,15 +521,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -525,142 +539,163 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -984,243 +1019,289 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:L14"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="27.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="9.57142857142857" customWidth="1"/>
+    <col min="1" max="1" width="32.1428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5714285714286" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.7142857142857" style="1"/>
+    <col min="5" max="6" width="13.1428571428571" style="1"/>
+    <col min="7" max="9" width="11.7142857142857" style="1"/>
+    <col min="10" max="10" width="13.1428571428571" style="1"/>
+    <col min="11" max="11" width="11.7142857142857" style="1"/>
+    <col min="12" max="12" width="10.5714285714286" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
-      <c r="B2" s="1">
+    <row r="1" spans="2:12">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D1" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E1" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F1" s="3">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G1" s="3">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H1" s="3">
         <v>6</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I1" s="3">
         <v>7</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J1" s="3">
         <v>8</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K1" s="3">
         <v>8</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L1" s="3">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>0</v>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <f>(C2+D2+E2+F2+G2+H2+I2+J2+K2+L2)/10</f>
+        <v>2982.8</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2904</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2774</v>
+      </c>
+      <c r="E2" s="6">
+        <v>3171</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2932</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3072</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3197</v>
+      </c>
+      <c r="I2" s="6">
+        <v>2845</v>
+      </c>
+      <c r="J2" s="6">
+        <v>2843</v>
+      </c>
+      <c r="K2" s="6">
+        <v>3122</v>
+      </c>
+      <c r="L2" s="6">
+        <v>2968</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>10002</v>
-      </c>
-      <c r="C3" s="2">
-        <v>10012</v>
-      </c>
-      <c r="D3" s="2">
-        <v>10250</v>
-      </c>
-      <c r="E3" s="2">
-        <v>9994</v>
-      </c>
-      <c r="F3" s="2">
-        <v>9847</v>
-      </c>
-      <c r="G3" s="2">
-        <v>9816</v>
-      </c>
-      <c r="H3" s="2">
-        <v>10319</v>
-      </c>
-      <c r="I3" s="2">
-        <v>10036</v>
-      </c>
-      <c r="J3" s="2">
-        <v>9854</v>
-      </c>
-      <c r="K3" s="2">
-        <v>9881</v>
-      </c>
-      <c r="L3" s="1">
-        <f>(B3+C3+D3+E3+F3+G3+H3+I3+J3+K3)/10</f>
-        <v>10001.1</v>
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <f>(C3+D3+E3+F3+G3+H3+I3+J3+K3+L3)/10</f>
+        <v>3933.6</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3717</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3349</v>
+      </c>
+      <c r="E3" s="6">
+        <v>3727</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3388</v>
+      </c>
+      <c r="G3" s="6">
+        <v>3577</v>
+      </c>
+      <c r="H3" s="6">
+        <v>4302</v>
+      </c>
+      <c r="I3" s="6">
+        <v>4371</v>
+      </c>
+      <c r="J3" s="6">
+        <v>4229</v>
+      </c>
+      <c r="K3" s="6">
+        <v>4233</v>
+      </c>
+      <c r="L3" s="6">
+        <v>4443</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3742</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4626</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4050</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3980</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3959</v>
-      </c>
-      <c r="G4" s="2">
-        <v>3756</v>
-      </c>
-      <c r="H4" s="2">
-        <v>4008</v>
-      </c>
-      <c r="I4" s="2">
-        <v>3655</v>
-      </c>
-      <c r="J4" s="2">
-        <v>3188</v>
-      </c>
-      <c r="K4" s="2">
-        <v>3804</v>
-      </c>
-      <c r="L4" s="1">
-        <f>(B4+C4+D4+E4+F4+G4+H4+I4+J4+K4)/10</f>
-        <v>3876.8</v>
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <f>(C4+D4+E4+F4+G4+H4+I4+J4+K4+L4)/10</f>
+        <v>5520.6</v>
+      </c>
+      <c r="C4" s="9">
+        <v>5677</v>
+      </c>
+      <c r="D4" s="9">
+        <v>4595</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5368</v>
+      </c>
+      <c r="F4" s="9">
+        <v>4627</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5569</v>
+      </c>
+      <c r="H4" s="9">
+        <v>5677</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5650</v>
+      </c>
+      <c r="J4" s="9">
+        <v>5904</v>
+      </c>
+      <c r="K4" s="9">
+        <v>6246</v>
+      </c>
+      <c r="L4" s="9">
+        <v>5893</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>8660</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8841</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8759</v>
-      </c>
-      <c r="E5" s="2">
-        <v>8686</v>
-      </c>
-      <c r="F5" s="2">
-        <v>8824</v>
-      </c>
-      <c r="G5" s="2">
-        <v>7846</v>
-      </c>
-      <c r="H5" s="2">
-        <v>8015</v>
-      </c>
-      <c r="I5" s="2">
-        <v>7778</v>
-      </c>
-      <c r="J5" s="2">
-        <v>7751</v>
-      </c>
-      <c r="K5" s="2">
-        <v>8174</v>
-      </c>
-      <c r="L5" s="1">
-        <f>(B5+C5+D5+E5+F5+G5+H5+I5+J5+K5)/10</f>
-        <v>8333.4</v>
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <f>(C5+D5+E5+F5+G5+H5+I5+J5+K5+L5)/10</f>
+        <v>8013.6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8132</v>
+      </c>
+      <c r="D5" s="6">
+        <v>7721</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8603</v>
+      </c>
+      <c r="F5" s="6">
+        <v>7795</v>
+      </c>
+      <c r="G5" s="6">
+        <v>8167</v>
+      </c>
+      <c r="H5" s="6">
+        <v>7997</v>
+      </c>
+      <c r="I5" s="6">
+        <v>7901</v>
+      </c>
+      <c r="J5" s="6">
+        <v>7919</v>
+      </c>
+      <c r="K5" s="6">
+        <v>7924</v>
+      </c>
+      <c r="L5" s="6">
+        <v>7977</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3409</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3328</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2987</v>
-      </c>
-      <c r="E6" s="2">
-        <v>3214</v>
-      </c>
-      <c r="F6" s="2">
-        <v>3396</v>
-      </c>
-      <c r="G6" s="2">
-        <v>3540</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2995</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2813</v>
-      </c>
-      <c r="J6" s="2">
-        <v>2781</v>
-      </c>
-      <c r="K6" s="2">
-        <v>3547</v>
-      </c>
-      <c r="L6" s="1">
-        <f>(B6+C6+D6+E6+F6+G6+H6+I6+J6+K6)/10</f>
-        <v>3201</v>
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <f>(C6+D6+E6+F6+G6+H6+I6+J6+K6+L6)/10</f>
+        <v>10003.8</v>
+      </c>
+      <c r="C6" s="6">
+        <v>10183</v>
+      </c>
+      <c r="D6" s="6">
+        <v>9634</v>
+      </c>
+      <c r="E6" s="6">
+        <v>9642</v>
+      </c>
+      <c r="F6" s="6">
+        <v>10055</v>
+      </c>
+      <c r="G6" s="6">
+        <v>10579</v>
+      </c>
+      <c r="H6" s="6">
+        <v>9914</v>
+      </c>
+      <c r="I6" s="6">
+        <v>9996</v>
+      </c>
+      <c r="J6" s="6">
+        <v>9887</v>
+      </c>
+      <c r="K6" s="6">
+        <v>10178</v>
+      </c>
+      <c r="L6" s="6">
+        <v>9970</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+    <row r="14" spans="8:10">
+      <c r="H14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
-    <row r="8" spans="7:7">
-      <c r="G8" s="2"/>
+    <row r="15" spans="8:10">
+      <c r="H15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
-    <row r="9" spans="7:7">
-      <c r="G9" s="1"/>
+    <row r="16" spans="8:10">
+      <c r="H16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
-    <row r="10" spans="7:7">
-      <c r="G10" s="1"/>
+    <row r="17" spans="8:10">
+      <c r="H17" s="3"/>
+      <c r="J17" s="3"/>
     </row>
-    <row r="11" spans="7:7">
-      <c r="G11" s="1"/>
+    <row r="18" spans="8:10">
+      <c r="H18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
-    <row r="12" spans="7:7">
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="7:7">
-      <c r="G14" s="2"/>
+    <row r="19" spans="2:6">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L6">
+    <sortState ref="A2:L6">
+      <sortCondition ref="B2"/>
+    </sortState>
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>